<commit_message>
affichage graphique dans Excel
</commit_message>
<xml_diff>
--- a/documents/statistiques/Statistiques_M1_2009.xlsx
+++ b/documents/statistiques/Statistiques_M1_2009.xlsx
@@ -157,6 +157,566 @@
   <dxfs count="0"/>
   <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr b="0" i="0" u="none" strike="noStrike">
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Lieu du stage</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout/>
+      </c:layout>
+      <c:pieChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9900"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:tx>
+            <c:strRef>
+              <c:f>Worksheet!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lieu du stage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Worksheet!$D$10:$D$14</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Le Mans</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sarthe</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pays de la Loire</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Etranger</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Worksheet!$E$10:$E$14</c:f>
+              <c:numCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins footer="0.3" header="0.3" r="0.7" l="0.7" t="0.75" b="0.75"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr b="0" i="0" u="none" strike="noStrike">
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Contenu du stage</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout/>
+      </c:layout>
+      <c:pieChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9900"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:tx>
+            <c:strRef>
+              <c:f>Worksheet!$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Contenu du stage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Worksheet!$D$16:$D$23</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>C#</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>COBOL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C++</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ASSEMBLEUR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ANDROID</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JEE</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DELPHI</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>PHP5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Worksheet!$E$16:$E$23</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins footer="0.3" header="0.3" r="0.7" l="0.7" t="0.75" b="0.75"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr b="0" i="0" u="none" strike="noStrike">
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Type du stage</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout/>
+      </c:layout>
+      <c:pieChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9900"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:tx>
+            <c:strRef>
+              <c:f>Worksheet!$B$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Type entreprise</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Worksheet!$D$25:$D$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Petite</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Moyenne</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Grande</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hors info</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Worksheet!$E$25:$E$28</c:f>
+              <c:numCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins footer="0.3" header="0.3" r="0.7" l="0.7" t="0.75" b="0.75"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr name="Chart 1" id="1025"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr name="Chart 2" id="2050"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr name="Chart 3" id="3075"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -554,7 +1114,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="C16" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
@@ -645,7 +1205,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="C25" t="s">
+      <c r="B25" t="s">
         <v>27</v>
       </c>
       <c r="D25" t="s">
@@ -704,5 +1264,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
amélioration de l'affichage des statistiques
</commit_message>
<xml_diff>
--- a/documents/statistiques/Statistiques_M1_2009.xlsx
+++ b/documents/statistiques/Statistiques_M1_2009.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>Statistiques stage M1 2009</t>
   </si>
@@ -71,37 +71,46 @@
     <t>C#</t>
   </si>
   <si>
+    <t>28.57 %</t>
+  </si>
+  <si>
+    <t>COBOL</t>
+  </si>
+  <si>
+    <t>64.29 %</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>0 %</t>
+  </si>
+  <si>
+    <t>ASSEMBLEUR</t>
+  </si>
+  <si>
+    <t>7.14 %</t>
+  </si>
+  <si>
+    <t>ANDROID</t>
+  </si>
+  <si>
+    <t>JEE</t>
+  </si>
+  <si>
+    <t>DELPHI</t>
+  </si>
+  <si>
+    <t>PHP5</t>
+  </si>
+  <si>
+    <t>Type entreprise</t>
+  </si>
+  <si>
+    <t>Petite</t>
+  </si>
+  <si>
     <t>100 %</t>
-  </si>
-  <si>
-    <t>COBOL</t>
-  </si>
-  <si>
-    <t>0 %</t>
-  </si>
-  <si>
-    <t>C++</t>
-  </si>
-  <si>
-    <t>ASSEMBLEUR</t>
-  </si>
-  <si>
-    <t>ANDROID</t>
-  </si>
-  <si>
-    <t>JEE</t>
-  </si>
-  <si>
-    <t>DELPHI</t>
-  </si>
-  <si>
-    <t>PHP5</t>
-  </si>
-  <si>
-    <t>Type entreprise</t>
-  </si>
-  <si>
-    <t>Petite</t>
   </si>
   <si>
     <t>Moyenne</t>
@@ -409,16 +418,16 @@
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>28</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1121,7 +1130,7 @@
         <v>17</v>
       </c>
       <c r="E16">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="G16" t="s">
         <v>18</v>
@@ -1132,7 +1141,7 @@
         <v>19</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G17" t="s">
         <v>20</v>
@@ -1146,109 +1155,109 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="D19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="D20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="D21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="D22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="D23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="B25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E25">
         <v>28</v>
       </c>
       <c r="G25" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="D26" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="D27" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="D28" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>